<commit_message>
Added functionality to save transactions to file
</commit_message>
<xml_diff>
--- a/Customers.xlsx
+++ b/Customers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming Projects\Mobile Banking App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C971EF-BB78-4C24-B865-2EB0380F2D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B328E1B-2748-4480-BA0F-339C32B82A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1B25E05E-0A38-408A-BD5F-74B7460FC059}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>OwnerName</t>
+  </si>
+  <si>
+    <t>Overdraft</t>
   </si>
   <si>
     <t>ABC company</t>
@@ -440,7 +443,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,10 +521,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{637AFE45-10D9-403E-ACA4-C4B04C259C24}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,7 +532,7 @@
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -548,13 +551,16 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -568,16 +574,19 @@
       <c r="F3">
         <v>21121</v>
       </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>2348</v>
@@ -587,6 +596,9 @@
       </c>
       <c r="F4">
         <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored code wherever required
</commit_message>
<xml_diff>
--- a/Customers.xlsx
+++ b/Customers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming Projects\Mobile Banking App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A58934-FA78-45C1-BA3E-AD822BE75018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E60C24-E42E-45EC-A312-96C7646F398E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1B25E05E-0A38-408A-BD5F-74B7460FC059}"/>
   </bookViews>
@@ -489,7 +489,7 @@
         <v>100136144</v>
       </c>
       <c r="F3" s="0">
-        <v>2300</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="4">
@@ -526,7 +526,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,10 +574,10 @@
         <v>900113678</v>
       </c>
       <c r="F3" s="0">
-        <v>-4000</v>
+        <v>2000</v>
       </c>
       <c r="G3" s="0">
-        <v>4000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">

</xml_diff>